<commit_message>
End to end data and tech asset threat model, with risk output creation in docker
</commit_message>
<xml_diff>
--- a/output/tags.xlsx
+++ b/output/tags.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="DfE SSPHP Threat Model" sheetId="2" r:id="rId4"/>
+    <sheet name="Some Example Application" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Element</t>
   </si>
@@ -22,13 +22,40 @@
     <t>azure</t>
   </si>
   <si>
-    <t>azure-function-app</t>
+    <t>azure-app-service</t>
+  </si>
+  <si>
+    <t>azure-container-app</t>
   </si>
   <si>
     <t>azure-key-vault</t>
   </si>
   <si>
-    <t>codeql</t>
+    <t>azure-redis-cache</t>
+  </si>
+  <si>
+    <t>azure-storage</t>
+  </si>
+  <si>
+    <t>bank-account-details</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>client-application-code</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>function</t>
   </si>
   <si>
     <t>git</t>
@@ -37,76 +64,100 @@
     <t>github</t>
   </si>
   <si>
-    <t>github-actions</t>
-  </si>
-  <si>
-    <t>o365</t>
-  </si>
-  <si>
-    <t>splunk</t>
-  </si>
-  <si>
-    <t>CodeQL Code Inspection</t>
+    <t>html</t>
+  </si>
+  <si>
+    <t>internal</t>
+  </si>
+  <si>
+    <t>javascript</t>
+  </si>
+  <si>
+    <t>job-information</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t>keyvault</t>
+  </si>
+  <si>
+    <t>payment-details</t>
+  </si>
+  <si>
+    <t>pci</t>
+  </si>
+  <si>
+    <t>pii</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>ruby</t>
+  </si>
+  <si>
+    <t>s184d01-comp-complete-app</t>
+  </si>
+  <si>
+    <t>s184d01-comp-complete-app-worker</t>
+  </si>
+  <si>
+    <t>s184d01-comp-tfvars</t>
+  </si>
+  <si>
+    <t>s184d01-compdefault</t>
+  </si>
+  <si>
+    <t>school-data</t>
+  </si>
+  <si>
+    <t>secrets</t>
+  </si>
+  <si>
+    <t>secrets-and-api-keys</t>
+  </si>
+  <si>
+    <t>sensitive</t>
+  </si>
+  <si>
+    <t>server-application-code</t>
+  </si>
+  <si>
+    <t>serverless</t>
+  </si>
+  <si>
+    <t>ssphp-metrics</t>
+  </si>
+  <si>
+    <t>ssphp-metrics-rust-p3sha</t>
+  </si>
+  <si>
+    <t>student-pii</t>
+  </si>
+  <si>
+    <t>teacher-pii</t>
+  </si>
+  <si>
+    <t>tfstatel95cd</t>
+  </si>
+  <si>
+    <t>tfstatep3sha</t>
+  </si>
+  <si>
+    <t>vault</t>
+  </si>
+  <si>
+    <t>vulnerable-children-data</t>
+  </si>
+  <si>
+    <t>SSPHP-Metrics</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>GitHub Actions Build Pipeline</t>
-  </si>
-  <si>
-    <t>Sourcecode Repository Traffic</t>
-  </si>
-  <si>
-    <t>Function App Push</t>
-  </si>
-  <si>
-    <t>Code Inspection Platform Traffic</t>
-  </si>
-  <si>
-    <t>GitHub Sourcecode Repository</t>
-  </si>
-  <si>
-    <t>Key Vault</t>
-  </si>
-  <si>
-    <t>Rust Function App</t>
-  </si>
-  <si>
-    <t>Send data to Splunk</t>
-  </si>
-  <si>
-    <t>Retrieve keys</t>
-  </si>
-  <si>
-    <t>Build Pipeline Traffic</t>
-  </si>
-  <si>
-    <t>API Calls to Services</t>
-  </si>
-  <si>
-    <t>Splunk</t>
-  </si>
-  <si>
-    <t>Various service REST endpoints</t>
-  </si>
-  <si>
-    <t>Secrets and API Keys</t>
-  </si>
-  <si>
-    <t>Sourcecode</t>
-  </si>
-  <si>
-    <t>Splunk data</t>
-  </si>
-  <si>
-    <t>Azure Trust Boundary</t>
-  </si>
-  <si>
-    <t>GitHub Trust Boundary</t>
-  </si>
-  <si>
-    <t>Splunk Trust Boundary</t>
+    <t>SSPHP-Metrics-rust-p3sha</t>
   </si>
 </sst>
 </file>
@@ -459,7 +510,7 @@
   </sheetViews>
   <cols>
     <col customWidth="true" max="1" min="1" width="60"/>
-    <col customWidth="true" max="10" min="2" width="35"/>
+    <col customWidth="true" max="45" min="2" width="35"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -493,160 +544,642 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -654,85 +1187,292 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -740,16 +1480,57 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -759,107 +1540,107 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1" t="s">
-        <v>11</v>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +1650,7 @@
     <oddFooter>&amp;C&amp;F</oddFooter>
     <evenHeader>&amp;L&amp;P</evenHeader>
     <evenFooter>&amp;L&amp;D&amp;R&amp;T</evenFooter>
-    <firstHeader>&amp;Tag Matrix &amp;"-,DfE SSPHP Threat Model"Bold&amp;"-,Regular"Summary+000A&amp;D</firstHeader>
+    <firstHeader>&amp;Tag Matrix &amp;"-,Some Example Application"Bold&amp;"-,Regular"Summary+000A&amp;D</firstHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix CodeQL issues: 20-36 - replace the jinja encoding with the value required in yaml - keeping the escape logic run by jinja
</commit_message>
<xml_diff>
--- a/output/tags.xlsx
+++ b/output/tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Element</t>
   </si>
@@ -80,6 +80,21 @@
   </si>
   <si>
     <t>keyvault</t>
+  </si>
+  <si>
+    <t>microsoft.app/containerapps</t>
+  </si>
+  <si>
+    <t>microsoft.cache/redis</t>
+  </si>
+  <si>
+    <t>microsoft.keyvault/vaults</t>
+  </si>
+  <si>
+    <t>microsoft.storage/storageaccounts</t>
+  </si>
+  <si>
+    <t>microsoft.web/sites</t>
   </si>
   <si>
     <t>payment-details</t>
@@ -504,7 +519,7 @@
   </sheetViews>
   <cols>
     <col customWidth="true" max="1" min="1" width="60"/>
-    <col customWidth="true" max="45" min="2" width="35"/>
+    <col customWidth="true" max="50" min="2" width="35"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -643,17 +658,32 @@
       <c r="AS1" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="AT1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -673,19 +703,21 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+      <c r="W2" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
@@ -698,17 +730,22 @@
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -728,20 +765,22 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="W3" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
+      <c r="AH3" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
@@ -753,18 +792,23 @@
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
       <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -782,57 +826,64 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
+      <c r="Y4" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
-      <c r="AD4" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
-      <c r="AG4" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
+      <c r="AI4" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
+      <c r="AL4" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
-      <c r="AR4" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AR4" s="1"/>
       <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -847,21 +898,23 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
+      <c r="X5" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
-      <c r="AE5" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
+      <c r="AJ5" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
@@ -871,18 +924,23 @@
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -900,12 +958,14 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
+      <c r="Y6" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
@@ -913,35 +973,40 @@
       <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
-      <c r="AG6" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR6" s="1"/>
       <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -954,7 +1019,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -968,7 +1033,9 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
+      <c r="AA7" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -978,37 +1045,42 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
-      <c r="AK7" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AK7" s="1"/>
       <c r="AL7" s="1"/>
-      <c r="AM7" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
-      <c r="AP7" s="1"/>
+      <c r="AP7" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
+      <c r="AR7" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1026,7 +1098,9 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
@@ -1042,30 +1116,35 @@
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
-      <c r="AP8" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
       <c r="AR8" s="1"/>
       <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1083,7 +1162,9 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="Z9" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
@@ -1100,11 +1181,16 @@
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
       <c r="AP9" s="1"/>
-      <c r="AQ9" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AQ9" s="1"/>
       <c r="AR9" s="1"/>
       <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -1120,25 +1206,25 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -1166,13 +1252,18 @@
       <c r="AQ10" s="1"/>
       <c r="AR10" s="1"/>
       <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1185,7 +1276,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1194,21 +1285,21 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
+      <c r="AE11" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
@@ -1223,13 +1314,18 @@
       <c r="AQ11" s="1"/>
       <c r="AR11" s="1"/>
       <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1237,14 +1333,14 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1255,42 +1351,47 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
+      <c r="AB12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
-      <c r="AI12" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
       <c r="AM12" s="1"/>
-      <c r="AN12" s="1"/>
+      <c r="AN12" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
       <c r="AR12" s="1"/>
       <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1303,14 +1404,14 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -1325,14 +1426,14 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
-      <c r="AF13" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
+      <c r="AK13" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AL13" s="1"/>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
@@ -1341,18 +1442,23 @@
       <c r="AQ13" s="1"/>
       <c r="AR13" s="1"/>
       <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1371,7 +1477,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -1384,26 +1490,31 @@
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
-      <c r="AH14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI14" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
-      <c r="AM14" s="1"/>
-      <c r="AN14" s="1"/>
+      <c r="AM14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AO14" s="1"/>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
       <c r="AR14" s="1"/>
       <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1416,15 +1527,15 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -1436,36 +1547,41 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
+      <c r="AF15" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
-      <c r="AJ15" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
-      <c r="AO15" s="1"/>
+      <c r="AO15" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
       <c r="AR15" s="1"/>
       <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1478,7 +1594,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1491,40 +1607,45 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-      <c r="Y16" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
+      <c r="AD16" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
-      <c r="AI16" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
       <c r="AR16" s="1"/>
-      <c r="AS16" s="1"/>
+      <c r="AS16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1537,7 +1658,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1550,40 +1671,45 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
-      <c r="Y17" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
+      <c r="AD17" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
-      <c r="AI17" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
       <c r="AL17" s="1"/>
       <c r="AM17" s="1"/>
-      <c r="AN17" s="1"/>
-      <c r="AO17" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AN17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO17" s="1"/>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
       <c r="AR17" s="1"/>
       <c r="AS17" s="1"/>
+      <c r="AT17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1596,7 +1722,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1609,32 +1735,37 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
-      <c r="Y18" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
+      <c r="AD18" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
-      <c r="AI18" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
       <c r="AM18" s="1"/>
-      <c r="AN18" s="1"/>
+      <c r="AN18" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="AO18" s="1"/>
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
       <c r="AR18" s="1"/>
-      <c r="AS18" s="1" t="s">
-        <v>45</v>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>